<commit_message>
add pão sirio e bolo de banana
</commit_message>
<xml_diff>
--- a/extras/planilha_ingredientes.xlsx
+++ b/extras/planilha_ingredientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\GitHub\receitas\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4452EF-2F7F-4038-AAD5-DD1AFAA03804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C1001A-4BE0-4FB2-A2E0-E91676EFC6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{B4274CAD-A22C-4886-982B-FF926DB21338}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{B4274CAD-A22C-4886-982B-FF926DB21338}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingredientes" sheetId="1" r:id="rId1"/>
@@ -37,31 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>kg de farinha de trigo</t>
-  </si>
-  <si>
-    <t>ml de leite morno</t>
-  </si>
-  <si>
-    <t>ml de água</t>
-  </si>
-  <si>
-    <t>ml de óleo</t>
-  </si>
-  <si>
-    <t>colheres de sopa de margarina</t>
-  </si>
-  <si>
-    <t>colher de sopa de açúcar</t>
-  </si>
-  <si>
-    <t>colher de sopa de sal</t>
-  </si>
-  <si>
-    <t>g de fermento seco</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>qtd</t>
   </si>
@@ -69,49 +45,49 @@
     <t>ingrediente</t>
   </si>
   <si>
-    <t>sal a gosto</t>
-  </si>
-  <si>
-    <t>limões taiti</t>
-  </si>
-  <si>
-    <t>cebola picada</t>
-  </si>
-  <si>
-    <t>tomate grande picado</t>
-  </si>
-  <si>
-    <t>g de carne moída</t>
-  </si>
-  <si>
-    <t>Misture a farinha de trigo, açúcar, sal, margarina, fermento, óleo, leite e água.</t>
-  </si>
-  <si>
-    <t>Agora é só sovar por pelo menos 10 minutos.</t>
-  </si>
-  <si>
-    <t>Separe em porções de 50 gramas e faça bolinhas.</t>
-  </si>
-  <si>
-    <t>Deixe descansar por 20 minutos até as bolinhas desenvolverem.</t>
-  </si>
-  <si>
-    <t>Para o recheio misture a carne moída, cebola, tomate, cheiro verde, suco de limão e sal a gosto.</t>
-  </si>
-  <si>
-    <t>Misture bem e deixe em uma peneira para escorrer o excesso de líquido.</t>
-  </si>
-  <si>
-    <t>Abra as bolinhas e recheie com carne moída.</t>
-  </si>
-  <si>
-    <t>Leve ao forno a 250 graus por aproximadamente 15 minutos.</t>
-  </si>
-  <si>
     <t>Preparo</t>
   </si>
   <si>
-    <t>O importante dessa esfiha é assar em temperatura alta por um curto espaço de tempo.</t>
+    <t>bananas maduras amassadas</t>
+  </si>
+  <si>
+    <t>ovos</t>
+  </si>
+  <si>
+    <t>xícara de açúcar</t>
+  </si>
+  <si>
+    <t>xícara de óleo vegetal</t>
+  </si>
+  <si>
+    <t>xícara de aveia em flocos</t>
+  </si>
+  <si>
+    <t>xícara de farinha de trigo</t>
+  </si>
+  <si>
+    <t>colher de sopa de canela em pó</t>
+  </si>
+  <si>
+    <t>colher de sopa de fermento em pó</t>
+  </si>
+  <si>
+    <t>Pré-aqueça o forno a 180°C e unte uma forma com margarina e farinha de trigo.</t>
+  </si>
+  <si>
+    <t>Em uma tigela grande, misture as bananas amassadas, os ovos, o açúcar e o óleo até obter uma mistura homogênea.</t>
+  </si>
+  <si>
+    <t>Adicione a aveia, a farinha de trigo e a canela em pó e misture bem.</t>
+  </si>
+  <si>
+    <t>Adicione o fermento em pó e mexa suavemente até incorporar à massa.</t>
+  </si>
+  <si>
+    <t>Despeje a massa na forma untada e leve ao forno por cerca de 30 a 40 minutos, ou até que o bolo esteja dourado e assado.</t>
+  </si>
+  <si>
+    <t>Retire do forno e deixe esfriar antes de servir.</t>
   </si>
 </sst>
 </file>
@@ -483,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54BAF34-FCA5-4D9E-86CF-F2FADBC4D557}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,70 +471,70 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A2&amp;"""&gt;"&amp;A2&amp;"&lt;/span&gt; "&amp;B2&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="1"&gt;1&lt;/span&gt; kg de farinha de trigo&lt;/li&gt;</v>
+        <f t="shared" ref="D2:D9" si="0">"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A2&amp;"""&gt;"&amp;A2&amp;"&lt;/span&gt; "&amp;B2&amp;"&lt;/li&gt;"</f>
+        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="3"&gt;3&lt;/span&gt; bananas maduras amassadas&lt;/li&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>350</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A3&amp;"""&gt;"&amp;A3&amp;"&lt;/span&gt; "&amp;B3&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="350"&gt;350&lt;/span&gt; ml de leite morno&lt;/li&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="2"&gt;2&lt;/span&gt; ovos&lt;/li&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>250</v>
+        <v>0.5</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D4" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A4&amp;"""&gt;"&amp;A4&amp;"&lt;/span&gt; "&amp;B4&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="250"&gt;250&lt;/span&gt; ml de água&lt;/li&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="0.5"&gt;0.5&lt;/span&gt; xícara de açúcar&lt;/li&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>150</v>
+        <v>0.5</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D5" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A5&amp;"""&gt;"&amp;A5&amp;"&lt;/span&gt; "&amp;B5&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="150"&gt;150&lt;/span&gt; ml de óleo&lt;/li&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="0.5"&gt;0.5&lt;/span&gt; xícara de óleo vegetal&lt;/li&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D6" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A6&amp;"""&gt;"&amp;A6&amp;"&lt;/span&gt; "&amp;B6&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="2"&gt;2&lt;/span&gt; colheres de sopa de margarina&lt;/li&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="1"&gt;1&lt;/span&gt; xícara de aveia em flocos&lt;/li&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,92 +542,35 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A7&amp;"""&gt;"&amp;A7&amp;"&lt;/span&gt; "&amp;B7&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="1"&gt;1&lt;/span&gt; colher de sopa de açúcar&lt;/li&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="1"&gt;1&lt;/span&gt; xícara de farinha de trigo&lt;/li&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D8" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A8&amp;"""&gt;"&amp;A8&amp;"&lt;/span&gt; "&amp;B8&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="1.5"&gt;1.5&lt;/span&gt; colher de sopa de sal&lt;/li&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="1"&gt;1&lt;/span&gt; colher de sopa de canela em pó&lt;/li&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
       <c r="D9" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A9&amp;"""&gt;"&amp;A9&amp;"&lt;/span&gt; "&amp;B9&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="10"&gt;10&lt;/span&gt; g de fermento seco&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>600</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A11&amp;"""&gt;"&amp;A11&amp;"&lt;/span&gt; "&amp;B11&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="600"&gt;600&lt;/span&gt; g de carne moída&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A12&amp;"""&gt;"&amp;A12&amp;"&lt;/span&gt; "&amp;B12&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="1"&gt;1&lt;/span&gt; tomate grande picado&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A13&amp;"""&gt;"&amp;A13&amp;"&lt;/span&gt; "&amp;B13&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="1"&gt;1&lt;/span&gt; cebola picada&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A14&amp;"""&gt;"&amp;A14&amp;"&lt;/span&gt; "&amp;B14&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="2"&gt;2&lt;/span&gt; limões taiti&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="str">
-        <f>"&lt;li&gt;&lt;span class=""qtd"" data-qtd="""&amp;A15&amp;"""&gt;"&amp;A15&amp;"&lt;/span&gt; "&amp;B15&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;&lt;span class="qtd" data-qtd=""&gt;&lt;/span&gt; sal a gosto&lt;/li&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;&lt;span class="qtd" data-qtd="1"&gt;1&lt;/span&gt; colher de sopa de fermento em pó&lt;/li&gt;</v>
       </c>
     </row>
   </sheetData>
@@ -662,7 +581,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8F168F-3530-47B3-B087-D797BF43BCB5}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -674,88 +593,61 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" t="str">
         <f>"&lt;li&gt;"&amp;A2&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;Misture a farinha de trigo, açúcar, sal, margarina, fermento, óleo, leite e água.&lt;/li&gt;</v>
+        <v>&lt;li&gt;Pré-aqueça o forno a 180°C e unte uma forma com margarina e farinha de trigo.&lt;/li&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B10" si="0">"&lt;li&gt;"&amp;A3&amp;"&lt;/li&gt;"</f>
-        <v>&lt;li&gt;Agora é só sovar por pelo menos 10 minutos.&lt;/li&gt;</v>
+        <f>"&lt;li&gt;"&amp;A3&amp;"&lt;/li&gt;"</f>
+        <v>&lt;li&gt;Em uma tigela grande, misture as bananas amassadas, os ovos, o açúcar e o óleo até obter uma mistura homogênea.&lt;/li&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;li&gt;Separe em porções de 50 gramas e faça bolinhas.&lt;/li&gt;</v>
+        <f t="shared" ref="B4:B7" si="0">"&lt;li&gt;"&amp;A4&amp;"&lt;/li&gt;"</f>
+        <v>&lt;li&gt;Adicione a aveia, a farinha de trigo e a canela em pó e misture bem.&lt;/li&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;li&gt;Deixe descansar por 20 minutos até as bolinhas desenvolverem.&lt;/li&gt;</v>
+        <v>&lt;li&gt;Adicione o fermento em pó e mexa suavemente até incorporar à massa.&lt;/li&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;li&gt;Para o recheio misture a carne moída, cebola, tomate, cheiro verde, suco de limão e sal a gosto.&lt;/li&gt;</v>
+        <v>&lt;li&gt;Despeje a massa na forma untada e leve ao forno por cerca de 30 a 40 minutos, ou até que o bolo esteja dourado e assado.&lt;/li&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;li&gt;Misture bem e deixe em uma peneira para escorrer o excesso de líquido.&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;li&gt;Abra as bolinhas e recheie com carne moída.&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;li&gt;Leve ao forno a 250 graus por aproximadamente 15 minutos.&lt;/li&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;li&gt;O importante dessa esfiha é assar em temperatura alta por um curto espaço de tempo.&lt;/li&gt;</v>
+        <v>&lt;li&gt;Retire do forno e deixe esfriar antes de servir.&lt;/li&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>